<commit_message>
Retrospectiva del sprint 2
</commit_message>
<xml_diff>
--- a/00 Administracion/Retrospectiva.xlsx
+++ b/00 Administracion/Retrospectiva.xlsx
@@ -5,14 +5,15 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PC5\Desktop\Semestre 11\Ingenieria de Software\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12120" windowHeight="4140"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12330" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Retrospectiva" sheetId="1" r:id="rId1"/>
+    <sheet name="Retrospectiva 1er Spring" sheetId="1" r:id="rId1"/>
+    <sheet name="Restrospectiva 2do Spring" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="24">
   <si>
     <t xml:space="preserve">COSAS QUE SALIERON BIEN </t>
   </si>
@@ -57,13 +58,52 @@
   </si>
   <si>
     <t>05. Comunicación por Facebook y "banquitas".</t>
+  </si>
+  <si>
+    <t xml:space="preserve">01. Definir el plan de trabajo claramente </t>
+  </si>
+  <si>
+    <t>02. Reasignación de equipos</t>
+  </si>
+  <si>
+    <t>01. Comunicación.</t>
+  </si>
+  <si>
+    <t>02. Falta de interes.</t>
+  </si>
+  <si>
+    <t>03. No superamos la curva de aprendizaje.</t>
+  </si>
+  <si>
+    <t>04. Falto crear la documentacion.</t>
+  </si>
+  <si>
+    <t>05. Incumplimiento del dailyScrum</t>
+  </si>
+  <si>
+    <t xml:space="preserve">plan de accion </t>
+  </si>
+  <si>
+    <t>subir los adelantos a github  o trello respectivamente, dependiendo de la naturaleza de los archivos</t>
+  </si>
+  <si>
+    <t>revisar facebook (conversacion de acuerdo al proyecto) dos veces por dia (5:00 pm y 9:00pm)</t>
+  </si>
+  <si>
+    <t>Creacion de bitacora invidual(columna personal en trello)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Todos los integrantes del equipo esten bien agregados a las plataformas de trabajo </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Multa ($50.00) por incumpliento de tareas inviduales asignas por el equipo interno (web y movil). y/o inasistencia al dailyscrum </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -90,6 +130,21 @@
       <name val="Bodoni MT"/>
       <family val="1"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="16"/>
+      <color rgb="FF000000"/>
+      <name val="Bodoni MT"/>
+      <family val="1"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -99,7 +154,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -144,15 +199,59 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -163,15 +262,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -179,6 +269,24 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -462,149 +570,149 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K10" sqref="K10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A10" sqref="A10:H14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="11.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:8" ht="21.75" thickBot="1">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
-      <c r="H1" s="4"/>
-    </row>
-    <row r="2" spans="1:8" ht="21" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="5" t="s">
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
+      <c r="H1" s="9"/>
+    </row>
+    <row r="2" spans="1:8" ht="21" thickBot="1">
+      <c r="A2" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="6"/>
-      <c r="C2" s="6"/>
-      <c r="D2" s="6"/>
-      <c r="E2" s="6"/>
-      <c r="F2" s="6"/>
-      <c r="G2" s="6"/>
-      <c r="H2" s="7"/>
-    </row>
-    <row r="3" spans="1:8" ht="21" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="5" t="s">
+      <c r="B2" s="5"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
+      <c r="G2" s="5"/>
+      <c r="H2" s="6"/>
+    </row>
+    <row r="3" spans="1:8" ht="21" thickBot="1">
+      <c r="A3" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="6"/>
-      <c r="C3" s="6"/>
-      <c r="D3" s="6"/>
-      <c r="E3" s="6"/>
-      <c r="F3" s="6"/>
-      <c r="G3" s="6"/>
-      <c r="H3" s="7"/>
-    </row>
-    <row r="4" spans="1:8" ht="21" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="5" t="s">
+      <c r="B3" s="5"/>
+      <c r="C3" s="5"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="5"/>
+      <c r="F3" s="5"/>
+      <c r="G3" s="5"/>
+      <c r="H3" s="6"/>
+    </row>
+    <row r="4" spans="1:8" ht="21" thickBot="1">
+      <c r="A4" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="6"/>
-      <c r="C4" s="6"/>
-      <c r="D4" s="6"/>
-      <c r="E4" s="6"/>
-      <c r="F4" s="6"/>
-      <c r="G4" s="6"/>
-      <c r="H4" s="7"/>
-    </row>
-    <row r="5" spans="1:8" ht="21" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="5" t="s">
+      <c r="B4" s="5"/>
+      <c r="C4" s="5"/>
+      <c r="D4" s="5"/>
+      <c r="E4" s="5"/>
+      <c r="F4" s="5"/>
+      <c r="G4" s="5"/>
+      <c r="H4" s="6"/>
+    </row>
+    <row r="5" spans="1:8" ht="21" thickBot="1">
+      <c r="A5" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="6"/>
-      <c r="C5" s="6"/>
-      <c r="D5" s="6"/>
-      <c r="E5" s="6"/>
-      <c r="F5" s="6"/>
-      <c r="G5" s="6"/>
-      <c r="H5" s="7"/>
-    </row>
-    <row r="6" spans="1:8" ht="21" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="5" t="s">
+      <c r="B5" s="5"/>
+      <c r="C5" s="5"/>
+      <c r="D5" s="5"/>
+      <c r="E5" s="5"/>
+      <c r="F5" s="5"/>
+      <c r="G5" s="5"/>
+      <c r="H5" s="6"/>
+    </row>
+    <row r="6" spans="1:8" ht="21" thickBot="1">
+      <c r="A6" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="6"/>
-      <c r="C6" s="6"/>
-      <c r="D6" s="6"/>
-      <c r="E6" s="6"/>
-      <c r="F6" s="6"/>
-      <c r="G6" s="6"/>
-      <c r="H6" s="7"/>
-    </row>
-    <row r="9" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="10" spans="1:8" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="2" t="s">
+      <c r="B6" s="5"/>
+      <c r="C6" s="5"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="5"/>
+      <c r="F6" s="5"/>
+      <c r="G6" s="5"/>
+      <c r="H6" s="6"/>
+    </row>
+    <row r="9" spans="1:8" ht="15.75" thickBot="1"/>
+    <row r="10" spans="1:8" ht="21.75" thickBot="1">
+      <c r="A10" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="B10" s="3"/>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
-      <c r="F10" s="3"/>
-      <c r="G10" s="3"/>
-      <c r="H10" s="4"/>
-    </row>
-    <row r="11" spans="1:8" ht="21" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="5" t="s">
+      <c r="B10" s="8"/>
+      <c r="C10" s="8"/>
+      <c r="D10" s="8"/>
+      <c r="E10" s="8"/>
+      <c r="F10" s="8"/>
+      <c r="G10" s="8"/>
+      <c r="H10" s="9"/>
+    </row>
+    <row r="11" spans="1:8" ht="21" thickBot="1">
+      <c r="A11" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B11" s="6"/>
-      <c r="C11" s="6"/>
-      <c r="D11" s="6"/>
-      <c r="E11" s="6"/>
-      <c r="F11" s="6"/>
-      <c r="G11" s="6"/>
-      <c r="H11" s="7"/>
-    </row>
-    <row r="12" spans="1:8" ht="69" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="8" t="s">
+      <c r="B11" s="5"/>
+      <c r="C11" s="5"/>
+      <c r="D11" s="5"/>
+      <c r="E11" s="5"/>
+      <c r="F11" s="5"/>
+      <c r="G11" s="5"/>
+      <c r="H11" s="6"/>
+    </row>
+    <row r="12" spans="1:8" ht="69" customHeight="1" thickBot="1">
+      <c r="A12" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="B12" s="9"/>
-      <c r="C12" s="9"/>
-      <c r="D12" s="9"/>
-      <c r="E12" s="9"/>
-      <c r="F12" s="9"/>
-      <c r="G12" s="9"/>
-      <c r="H12" s="10"/>
-    </row>
-    <row r="13" spans="1:8" ht="49.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="8" t="s">
+      <c r="B12" s="11"/>
+      <c r="C12" s="11"/>
+      <c r="D12" s="11"/>
+      <c r="E12" s="11"/>
+      <c r="F12" s="11"/>
+      <c r="G12" s="11"/>
+      <c r="H12" s="12"/>
+    </row>
+    <row r="13" spans="1:8" ht="49.5" customHeight="1" thickBot="1">
+      <c r="A13" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="B13" s="9"/>
-      <c r="C13" s="9"/>
-      <c r="D13" s="9"/>
-      <c r="E13" s="9"/>
-      <c r="F13" s="9"/>
-      <c r="G13" s="9"/>
-      <c r="H13" s="10"/>
-    </row>
-    <row r="14" spans="1:8" ht="21" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="5" t="s">
+      <c r="B13" s="11"/>
+      <c r="C13" s="11"/>
+      <c r="D13" s="11"/>
+      <c r="E13" s="11"/>
+      <c r="F13" s="11"/>
+      <c r="G13" s="11"/>
+      <c r="H13" s="12"/>
+    </row>
+    <row r="14" spans="1:8" ht="21" thickBot="1">
+      <c r="A14" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B14" s="6"/>
-      <c r="C14" s="6"/>
-      <c r="D14" s="6"/>
-      <c r="E14" s="6"/>
-      <c r="F14" s="6"/>
-      <c r="G14" s="6"/>
-      <c r="H14" s="7"/>
-    </row>
-    <row r="16" spans="1:8" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="B14" s="5"/>
+      <c r="C14" s="5"/>
+      <c r="D14" s="5"/>
+      <c r="E14" s="5"/>
+      <c r="F14" s="5"/>
+      <c r="G14" s="5"/>
+      <c r="H14" s="6"/>
+    </row>
+    <row r="16" spans="1:8" ht="20.25">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
@@ -631,4 +739,206 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J23"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G32" sqref="G32"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:10" ht="21.75" thickBot="1">
+      <c r="A1" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
+      <c r="H1" s="9"/>
+    </row>
+    <row r="2" spans="1:10" ht="21" thickBot="1">
+      <c r="A2" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" s="5"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
+      <c r="G2" s="5"/>
+      <c r="H2" s="6"/>
+    </row>
+    <row r="3" spans="1:10" ht="21" thickBot="1">
+      <c r="A3" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="5"/>
+      <c r="C3" s="5"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="5"/>
+      <c r="F3" s="5"/>
+      <c r="G3" s="5"/>
+      <c r="H3" s="6"/>
+    </row>
+    <row r="4" spans="1:10" ht="21" thickBot="1">
+      <c r="A4" s="4"/>
+      <c r="B4" s="5"/>
+      <c r="C4" s="5"/>
+      <c r="D4" s="5"/>
+      <c r="E4" s="5"/>
+      <c r="F4" s="5"/>
+      <c r="G4" s="5"/>
+      <c r="H4" s="6"/>
+    </row>
+    <row r="5" spans="1:10" ht="20.25">
+      <c r="A5" s="16"/>
+      <c r="B5" s="17"/>
+      <c r="C5" s="17"/>
+      <c r="D5" s="17"/>
+      <c r="E5" s="17"/>
+      <c r="F5" s="17"/>
+      <c r="G5" s="17"/>
+      <c r="H5" s="18"/>
+    </row>
+    <row r="6" spans="1:10" ht="20.25">
+      <c r="A6" s="3"/>
+      <c r="B6" s="3"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3"/>
+      <c r="H6" s="3"/>
+    </row>
+    <row r="7" spans="1:10">
+      <c r="J7" s="2"/>
+    </row>
+    <row r="9" spans="1:10" ht="15.75" thickBot="1"/>
+    <row r="10" spans="1:10" ht="21.75" thickBot="1">
+      <c r="A10" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="B10" s="8"/>
+      <c r="C10" s="8"/>
+      <c r="D10" s="8"/>
+      <c r="E10" s="8"/>
+      <c r="F10" s="8"/>
+      <c r="G10" s="8"/>
+      <c r="H10" s="9"/>
+    </row>
+    <row r="11" spans="1:10" ht="21" thickBot="1">
+      <c r="A11" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11" s="5"/>
+      <c r="C11" s="5"/>
+      <c r="D11" s="5"/>
+      <c r="E11" s="5"/>
+      <c r="F11" s="5"/>
+      <c r="G11" s="5"/>
+      <c r="H11" s="6"/>
+    </row>
+    <row r="12" spans="1:10" ht="21" thickBot="1">
+      <c r="A12" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="B12" s="11"/>
+      <c r="C12" s="11"/>
+      <c r="D12" s="11"/>
+      <c r="E12" s="11"/>
+      <c r="F12" s="11"/>
+      <c r="G12" s="11"/>
+      <c r="H12" s="12"/>
+    </row>
+    <row r="13" spans="1:10" ht="21" thickBot="1">
+      <c r="A13" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="B13" s="11"/>
+      <c r="C13" s="11"/>
+      <c r="D13" s="11"/>
+      <c r="E13" s="11"/>
+      <c r="F13" s="11"/>
+      <c r="G13" s="11"/>
+      <c r="H13" s="12"/>
+    </row>
+    <row r="14" spans="1:10" ht="21" thickBot="1">
+      <c r="A14" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B14" s="5"/>
+      <c r="C14" s="5"/>
+      <c r="D14" s="5"/>
+      <c r="E14" s="5"/>
+      <c r="F14" s="5"/>
+      <c r="G14" s="5"/>
+      <c r="H14" s="6"/>
+    </row>
+    <row r="15" spans="1:10" ht="21" thickBot="1">
+      <c r="A15" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="B15" s="14"/>
+      <c r="C15" s="14"/>
+      <c r="D15" s="14"/>
+      <c r="E15" s="14"/>
+      <c r="F15" s="14"/>
+      <c r="G15" s="14"/>
+      <c r="H15" s="15"/>
+    </row>
+    <row r="18" spans="1:10">
+      <c r="A18" t="s">
+        <v>18</v>
+      </c>
+      <c r="J18" s="2"/>
+    </row>
+    <row r="19" spans="1:10">
+      <c r="A19" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10">
+      <c r="A20" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10">
+      <c r="A21" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10">
+      <c r="A22" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10">
+      <c r="A23" t="s">
+        <v>23</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="11">
+    <mergeCell ref="A15:H15"/>
+    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="A2:H2"/>
+    <mergeCell ref="A3:H3"/>
+    <mergeCell ref="A4:H4"/>
+    <mergeCell ref="A5:H5"/>
+    <mergeCell ref="A10:H10"/>
+    <mergeCell ref="A11:H11"/>
+    <mergeCell ref="A12:H12"/>
+    <mergeCell ref="A13:H13"/>
+    <mergeCell ref="A14:H14"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>